<commit_message>
Finished outer walls WIP
</commit_message>
<xml_diff>
--- a/FreeCAD/Dimensions.xlsx
+++ b/FreeCAD/Dimensions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>Main Cottage</t>
   </si>
@@ -66,6 +66,15 @@
   </si>
   <si>
     <t>South External</t>
+  </si>
+  <si>
+    <t>Floor</t>
+  </si>
+  <si>
+    <t>External East Door Way</t>
+  </si>
+  <si>
+    <t>External Main Walls</t>
   </si>
 </sst>
 </file>
@@ -417,7 +426,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -529,36 +538,81 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D6">
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="E6">
-        <f>D6*N2</f>
-        <v>9520</v>
+        <f>D6*N1</f>
+        <v>4200</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>15</v>
+      </c>
+      <c r="E7">
+        <f>D7*N1</f>
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8">
+        <v>85</v>
+      </c>
+      <c r="E8">
+        <f>D8*N2</f>
+        <v>9520</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C9" t="s">
         <v>8</v>
       </c>
-      <c r="D7">
+      <c r="D9">
         <v>53</v>
       </c>
-      <c r="E7">
-        <f>D7*N2</f>
+      <c r="E9">
+        <f>D9*N2</f>
         <v>5936</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10">
+        <v>-22</v>
+      </c>
+      <c r="E10">
+        <f>D10*N1</f>
+        <v>-3080</v>
       </c>
     </row>
   </sheetData>

</xml_diff>